<commit_message>
Updated documentation for the summary excel workbooks Updated the traceroutes/parse_traceroute.php to resolve an issue
</commit_message>
<xml_diff>
--- a/performance reports/ibbs-query-metrics-combined.xlsx
+++ b/performance reports/ibbs-query-metrics-combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.abdul\Documents\Version Control\Git\sqlplus-query-metrics-ibbs\performance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2CABAC-CEEB-47F7-8885-EB132315EC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933FFDE4-CFD6-41B4-9C62-07F1D80DB5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2595" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42333,7 +42333,7 @@
   <dimension ref="A1:AX65"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>